<commit_message>
Finished everything - timer, olympiad ending, changed way of registration etc, fixed some bugs
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A49412-CEC9-43D4-B1E1-5E95647EB078}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +19,77 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Team1</t>
+  </si>
+  <si>
+    <t>Team2</t>
+  </si>
+  <si>
+    <t>Team3</t>
+  </si>
+  <si>
+    <t>Team4</t>
+  </si>
+  <si>
+    <t>Team5</t>
+  </si>
+  <si>
+    <t>Team6</t>
+  </si>
+  <si>
+    <t>Team7</t>
+  </si>
+  <si>
+    <t>Team8</t>
+  </si>
+  <si>
+    <t>Team9</t>
+  </si>
+  <si>
+    <t>Team10</t>
+  </si>
+  <si>
+    <t>Team11</t>
+  </si>
+  <si>
+    <t>Team12</t>
+  </si>
+  <si>
+    <t>Team13</t>
+  </si>
+  <si>
+    <t>Team14</t>
+  </si>
+  <si>
+    <t>Team15</t>
+  </si>
+  <si>
+    <t>Team16</t>
+  </si>
+  <si>
+    <t>Team17</t>
+  </si>
+  <si>
+    <t>Team18</t>
+  </si>
+  <si>
+    <t>Team19</t>
+  </si>
+  <si>
+    <t>Team20</t>
+  </si>
+  <si>
+    <t>Бали</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +97,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +137,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +426,787 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3">
+        <f xml:space="preserve"> B22*B2+C22*C2+D22*D2+E22*E2+F22*F2+G22*G2+H22*H2+I22*I2+J22*J2+K22*K2+L22*L2+M22*M2+N22*N2+O22*O2+P22*P2+Q22*Q2+R22*R2+S22*S2+T22*T2+U22*U2</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="3">
+        <f xml:space="preserve"> B22*B3+C22*C3+D22*D3+E22*E3+F22*F3+G22*G3+H22*H3+I22*I3+J22*J3+K22*K3+L22*L3+M22*M3+N22*N3+O22*O3+P22*P3+Q22*Q3+R22*R3+S22*S3+T22*T3+U22*U3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="3">
+        <f xml:space="preserve"> B22*B4+C22*C4+D22*D4+E22*E4+F22*F4+G22*G4+H22*H4+I22*I4+J22*J4+K22*K4+L22*L4+M22*M4+N22*N4+O22*O4+P22*P4+Q22*Q4+R22*R4+S22*S4+T22*T4+U22*U4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="3">
+        <f xml:space="preserve"> B22*B5+C22*C5+D22*D5+E22*E5+F22*F5+G22*G5+H22*H5+I22*I5+J22*J5+K22*K5+L22*L5+M22*M5+N22*N5+O22*O5+P22*P5+Q22*Q5+R22*R5+S22*S5+T22*T5+U22*U5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="3">
+        <f xml:space="preserve"> B22*B6+C22*C6+D22*D6+E22*E6+F22*F6+G22*G6+H22*H6+I22*I6+J22*J6+K22*K6+L22*L6+M22*M6+N22*N6+O22*O6+P22*P6+Q22*Q6+R22*R6+S22*S6+T22*T6+U22*U6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="3">
+        <f xml:space="preserve"> B22*B7+C22*C7+D22*D7+E22*E7+F22*F7+G22*G7+H22*H7+I22*I7+J22*J7+K22*K7+L22*L7+M22*M7+N22*N7+O22*O7+P22*P7+Q22*Q7+R22*R7+S22*S7+T22*T7+U22*U7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="3">
+        <f xml:space="preserve"> B22*B8+C22*C8+D22*D8+E22*E8+F22*F8+G22*G8+H22*H8+I22*I8+J22*J8+K22*K8+L22*L8+M22*M8+N22*N8+O22*O8+P22*P8+Q22*Q8+R22*R8+S22*S8+T22*T8+U22*U8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="3">
+        <f xml:space="preserve"> B22*B9+C22*C9+D22*D9+E22*E9+F22*F9+G22*G9+H22*H9+I22*I9+J22*J9+K22*K9+L22*L9+M22*M9+N22*N9+O22*O9+P22*P9+Q22*Q9+R22*R9+S22*S9+T22*T9+U22*U9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="3">
+        <f xml:space="preserve"> B22*B10+C22*C10+D22*D10+E22*E10+F22*F10+G22*G10+H22*H10+I22*I10+J22*J10+K22*K10+L22*L10+M22*M10+N22*N10+O22*O10+P22*P10+Q22*Q10+R22*R10+S22*S10+T22*T10+U22*U10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="3">
+        <f xml:space="preserve"> B22*B11+C22*C11+D22*D11+E22*E11+F22*F11+G22*G11+H22*H11+I22*I11+J22*J11+K22*K11+L22*L11+M22*M11+N22*N11+O22*O11+P22*P11+Q22*Q11+R22*R11+S22*S11+T22*T11+U22*U11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="3">
+        <f xml:space="preserve"> B22*B12+C22*C12+D22*D12+E22*E12+F22*F12+G22*G12+H22*H12+I22*I12+J22*J12+K22*K12+L22*L12+M22*M12+N22*N12+O22*O12+P22*P12+Q22*Q12+R22*R12+S22*S12+T22*T12+U22*U12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="3">
+        <f xml:space="preserve"> B22*B13+C22*C13+D22*D13+E22*E13+F22*F13+G22*G13+H22*H13+I22*I13+J22*J13+K22*K13+L22*L13+M22*M13+N22*N13+O22*O13+P22*P13+Q22*Q13+R22*R13+S22*S13+T22*T13+U22*U13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="3">
+        <f xml:space="preserve"> B22*B14+C22*C14+D22*D14+E22*E14+F22*F14+G22*G14+H22*H14+I22*I14+J22*J14+K22*K14+L22*L14+M22*M14+N22*N14+O22*O14+P22*P14+Q22*Q14+R22*R14+S22*S14+T22*T14+U22*U14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="3">
+        <f xml:space="preserve"> B22*B15+C22*C15+D22*D15+E22*E15+F22*F15+G22*G15+H22*H15+I22*I15+J22*J15+K22*K15+L22*L15+M22*M15+N22*N15+O22*O15+P22*P15+Q22*Q15+R22*R15+S22*S15+T22*T15+U22*U15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="3">
+        <f xml:space="preserve"> B22*B16+C22*C16+D22*D16+E22*E16+F22*F16+G22*G16+H22*H16+I22*I16+J22*J16+K22*K16+L22*L16+M22*M16+N22*N16+O22*O16+P22*P16+Q22*Q16+R22*R16+S22*S16+T22*T16+U22*U16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="3">
+        <f xml:space="preserve"> B22*B17+C22*C17+D22*D17+E22*E17+F22*F17+G22*G17+H22*H17+I22*I17+J22*J17+K22*K17+L22*L17+M22*M17+N22*N17+O22*O17+P22*P17+Q22*Q17+R22*R17+S22*S17+T22*T17+U22*U17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="3">
+        <f xml:space="preserve"> B22*B18+C22*C18+D22*D18+E22*E18+F22*F18+G22*G18+H22*H18+I22*I18+J22*J18+K22*K18+L22*L18+M22*M18+N22*N18+O22*O18+P22*P18+Q22*Q18+R22*R18+S22*S18+T22*T18+U22*U18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="3">
+        <f xml:space="preserve"> B22*B19+C22*C19+D22*D19+E22*E19+F22*F19+G22*G19+H22*H19+I22*I19+J22*J19+K22*K19+L22*L19+M22*M19+N22*N19+O22*O19+P22*P19+Q22*Q19+R22*R19+S22*S19+T22*T19+U22*U19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="3">
+        <f xml:space="preserve"> B22*B20+C22*C20+D22*D20+E22*E20+F22*F20+G22*G20+H22*H20+I22*I20+J22*J20+K22*K20+L22*L20+M22*M20+N22*N20+O22*O20+P22*P20+Q22*Q20+R22*R20+S22*S20+T22*T20+U22*U20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="3">
+        <f xml:space="preserve"> B22*B21+C22*C21+D22*D21+E22*E21+F22*F21+G22*G21+H22*H21+I22*I21+J22*J21+K22*K21+L22*L21+M22*M21+N22*N21+O22*O21+P22*P21+Q22*Q21+R22*R21+S22*S21+T22*T21+U22*U21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
+        <f xml:space="preserve"> 20 - SUM(B2:B21)</f>
+        <v>19</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" ref="C22:U22" si="0" xml:space="preserve"> 20 - SUM(C2:C21)</f>
+        <v>19</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="S22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="T22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="V3" formula="1"/>
+    <ignoredError sqref="B22:U22" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Separated back and front
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A49412-CEC9-43D4-B1E1-5E95647EB078}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EACF7-D0DE-4988-BA67-3F1F6DD84D07}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,69 +504,29 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
       <c r="V2" s="3">
         <f xml:space="preserve"> B22*B2+C22*C2+D22*D2+E22*E2+F22*F2+G22*G2+H22*H2+I22*I2+J22*J2+K22*K2+L22*L2+M22*M2+N22*N2+O22*O2+P22*P2+Q22*Q2+R22*R2+S22*S2+T22*T2+U22*U2</f>
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -1123,11 +1083,11 @@
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <f xml:space="preserve"> 20 - SUM(B2:B21)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" ref="C22:U22" si="0" xml:space="preserve"> 20 - SUM(C2:C21)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
@@ -1175,7 +1135,7 @@
       </c>
       <c r="O22" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" si="0"/>
@@ -1199,7 +1159,7 @@
       </c>
       <c r="U22" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated moderator and main moderator, added ability to stop moderators to check and give final results.
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EACF7-D0DE-4988-BA67-3F1F6DD84D07}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDCA4AA-FC5C-449E-9C2B-4E418F412AA8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,11 +504,19 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -526,7 +534,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="3">
         <f xml:space="preserve"> B22*B2+C22*C2+D22*D2+E22*E2+F22*F2+G22*G2+H22*H2+I22*I2+J22*J2+K22*K2+L22*L2+M22*M2+N22*N2+O22*O2+P22*P2+Q22*Q2+R22*R2+S22*S2+T22*T2+U22*U2</f>
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -562,29 +570,67 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
       <c r="V4" s="3">
         <f xml:space="preserve"> B22*B4+C22*C4+D22*D4+E22*E4+F22*F4+G22*G4+H22*H4+I22*I4+J22*J4+K22*K4+L22*L4+M22*M4+N22*N4+O22*O4+P22*P4+Q22*Q4+R22*R4+S22*S4+T22*T4+U22*U4</f>
-        <v>0</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -1083,83 +1129,83 @@
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <f xml:space="preserve"> 20 - SUM(B2:B21)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" ref="C22:U22" si="0" xml:space="preserve"> 20 - SUM(C2:C21)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U22" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>